<commit_message>
1.add menu and button tables 2.modify login and middleware func
</commit_message>
<xml_diff>
--- a/appinterfaces.xlsx
+++ b/appinterfaces.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="URL" sheetId="1" r:id="rId1"/>
     <sheet name="页面" sheetId="2" r:id="rId2"/>
+    <sheet name="菜单" sheetId="3" r:id="rId3"/>
+    <sheet name="按钮" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
   <si>
     <t>url通配符</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -170,11 +172,586 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>instance.views.interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vminstances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hostdetail.views.hostusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instance.views.inst_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instance.views.instusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/servers/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计接口1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/infrastructure/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instances/{\d}+/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>info/insts_status/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/storages/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/create/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/networks/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/network/1/bridge/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/interfaces/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/secrets/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/host/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>host</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/info/hostusage/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instance/1/bg51/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计接口3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/info/instusage/1/bg51/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计接口4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计接口5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/info/inst_status/1/bg51/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白名单</t>
+  </si>
+  <si>
+    <t>白名单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白名单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>白名单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面内权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按钮部分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servers_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>infrastructure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>createVM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/interfaces/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/login/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/logout/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/servers/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/infrastructure/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/host/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/create/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/storages/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/storage/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/network/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/interface/(\d+)/([\w\.\:]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/i18n/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vminstance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/instances/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/instance/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/console/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/secrets/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/info/hostusage/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/admin/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/info/instusage/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hostusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insts_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/info/insts_status/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/info/inst_status/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i18n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>方法名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>功能说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^login/?$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^logout/?$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登出页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跳转或者登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^servers/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servers_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过各种方式添加宿主机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servers_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>infrastructure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^infrastructure/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看宿主机资源使用情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>infrastructure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^host/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宿主机详细信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^create/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建虚拟机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^storages/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^storage/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计接口2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建存储目录和区域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建磁盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^networks/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建网络接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>network</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>instance.views.interface</t>
+    <t>network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^network/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定单块网卡的状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^interfaces/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^interface/(\d+)/([\w\.\:]+)/$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -182,11 +759,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Vminstances</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hostdetail.views.hostusage</t>
+    <t>interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^secrets/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^console/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hostusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/hostusage/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源查看</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -194,7 +811,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>instance.views.inst_status</t>
+    <t>insts_status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -202,7 +819,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>instance.views.instusage</t>
+    <t>inst_status</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -210,7 +827,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>i18n</t>
+    <t>instusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/insts_status/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/inst_status/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/instusage/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜单名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instances/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insterfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -218,242 +875,100 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>logout</t>
+    <t>/instance/1/bg021/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侧面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snapshots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>migrate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>destory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>viewer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instances/1/</t>
+  </si>
+  <si>
+    <t>button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>force shutdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shutdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>save</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suspend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>/servers/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计接口1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Infrastructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>servers</t>
+  </si>
+  <si>
+    <t>add connection</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>/infrastructure/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>instances</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/instances/{\d}+/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>info/insts_status/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/storages/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/create/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/networks/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/network/1/bridge/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/interfaces/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interfaces</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/secrets/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>secrets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/host/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>host</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/info/hostusage/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/instance/1/bg51/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计接口2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计接口3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/info/instusage/1/bg51/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计接口4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计接口5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/info/inst_status/1/bg51/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>权限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>白名单</t>
-  </si>
-  <si>
-    <t>白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>白名单</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>页面内权限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>否</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>部分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>超链接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>按钮部分</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>管理员</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>servers_list</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>infrastructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>createVM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interfaces</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/interfaces/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/login/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/logout/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/servers/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/infrastructure/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/host/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/create/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/storages/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/storage/(\d+)/([\w\-\.]+)/$</t>
+  </si>
+  <si>
+    <t>虚拟机的超链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>network</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -461,71 +976,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>^/network/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/interface/(\d+)/([\w\.\:]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/i18n/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Vminstance</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>secrets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/instances/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/instance/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/console/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/secrets/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>console</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hostusage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/info/hostusage/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/info/insts_status/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/info/inst_status/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/admin/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/info/instusage/(\d+)/([\w\-\.]+)/$</t>
+    <t>delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>viewer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -868,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -892,18 +1351,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -912,15 +1371,15 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -929,15 +1388,15 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -946,15 +1405,15 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -963,21 +1422,21 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G5" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -986,21 +1445,21 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1009,15 +1468,15 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1026,18 +1485,18 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -1049,12 +1508,12 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1063,15 +1522,15 @@
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>237</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -1080,15 +1539,15 @@
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -1097,15 +1556,15 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>236</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -1114,32 +1573,32 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
       <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
-        <v>38</v>
-      </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1148,15 +1607,15 @@
         <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1165,15 +1624,15 @@
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -1182,15 +1641,15 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -1199,29 +1658,29 @@
         <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E19" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
@@ -1230,49 +1689,49 @@
         <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="E21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1281,12 +1740,12 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1304,125 +1763,825 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>166</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
-        <v>78</v>
-      </c>
       <c r="F4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="C18" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>146</v>
+      </c>
+      <c r="B19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D21" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" t="s">
+        <v>157</v>
+      </c>
+      <c r="D22" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>170</v>
+      </c>
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+      <c r="C24" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" t="s">
+        <v>173</v>
+      </c>
+      <c r="E24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" t="s">
+        <v>177</v>
+      </c>
+      <c r="E25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" t="s">
+        <v>180</v>
+      </c>
+      <c r="C26" t="s">
+        <v>167</v>
+      </c>
+      <c r="E26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C29" t="s">
+        <v>191</v>
+      </c>
+      <c r="E29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" t="s">
+        <v>191</v>
+      </c>
+      <c r="D30" t="s">
+        <v>194</v>
+      </c>
+      <c r="E30" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>197</v>
+      </c>
+      <c r="B32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" t="s">
+        <v>191</v>
+      </c>
+      <c r="E32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>199</v>
+      </c>
+      <c r="B33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" t="s">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>214</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="C13" t="s">
+        <v>214</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" t="s">
+        <v>222</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C16" t="s">
+        <v>222</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" t="s">
+        <v>219</v>
+      </c>
+      <c r="C18" t="s">
+        <v>222</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C19" t="s">
+        <v>222</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" t="s">
+        <v>221</v>
+      </c>
+      <c r="C20" t="s">
+        <v>222</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="B7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="B9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.modify menu and button tables 2.modify html pages include js
</commit_message>
<xml_diff>
--- a/appinterfaces.xlsx
+++ b/appinterfaces.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="URL" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="257">
   <si>
     <t>url通配符</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -587,404 +587,469 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>servers_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过各种方式添加宿主机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servers_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>infrastructure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^infrastructure/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看宿主机资源使用情况</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>infrastructure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^host/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宿主机详细信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^create/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建虚拟机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^storages/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^storage/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设计接口2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建存储目录和区域</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建磁盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^networks/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建网络接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^network/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定单块网卡的状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^interfaces/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^interface/(\d+)/([\w\.\:]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^secrets/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>console</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^console/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hostusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/hostusage/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insts_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insts_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instusage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/insts_status/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/inst_status/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^info/instusage/(\d+)/([\w\-\.]+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜单名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instances/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insterfaces</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>secrets</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>overview</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侧面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>access</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>snapshots</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>statistics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>settings</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>migrate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>destory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>横向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>viewer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>force shutdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shutdown</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>save</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>suspend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/servers/</t>
+  </si>
+  <si>
+    <t>add connection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/infrastructure/</t>
+  </si>
+  <si>
+    <t>虚拟机的超链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>network</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^/networks/(\d+)/$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>viewer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pagename</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instance/1/bg021/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>edit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录行为</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>^login/?$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>servers_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>^servers/$</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>/info/insts_status/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/instances/1/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>instances</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>servers_list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>首页</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过各种方式添加宿主机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>servers_list</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>infrastructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^infrastructure/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看宿主机资源使用情况</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>infrastructure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^host/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>overview</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宿主机详细信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>overview</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^create/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建虚拟机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>create</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^storages/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^storage/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>设计接口2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建存储目录和区域</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建磁盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^networks/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>networks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建网络接口</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>network</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>network</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^network/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指定单块网卡的状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interfaces</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interfaces</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^interfaces/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^interface/(\d+)/([\w\.\:]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interface</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>secrets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>secrets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>post</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^secrets/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>console</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>console</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^console/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>get</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>hostusage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^info/hostusage/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>资源查看</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>insts_status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insts_status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inst_status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>inst_status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>instusage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>instusage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^info/insts_status/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^info/inst_status/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^info/instusage/(\d+)/([\w\-\.]+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>菜单名称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/instances/1/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>instances</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>storages</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insterfaces</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>secrets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>overview</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/instance/1/bg021/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>位置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>侧面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>power</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>access</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>snapshots</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>statistics</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>settings</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>migrate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>destory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>横向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>viewer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>url</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/instances/1/</t>
-  </si>
-  <si>
-    <t>button</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>force shutdown</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>shutdown</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>save</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>suspend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>start</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/servers/</t>
-  </si>
-  <si>
-    <t>add connection</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/infrastructure/</t>
-  </si>
-  <si>
-    <t>虚拟机的超链接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>network</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>^/networks/(\d+)/$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>edit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>viewer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -992,7 +1057,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1014,6 +1079,12 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1B1B1B"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1038,12 +1109,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1607,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s">
         <v>27</v>
@@ -1556,7 +1633,7 @@
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="E12" t="s">
         <v>84</v>
@@ -1763,10 +1840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1787,7 +1864,7 @@
         <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D1" t="s">
         <v>68</v>
@@ -1906,7 +1983,7 @@
         <v>128</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
         <v>130</v>
@@ -1920,301 +1997,328 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
       <c r="D15" t="s">
-        <v>134</v>
+        <v>245</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
         <v>137</v>
       </c>
       <c r="D17" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B18" t="s">
+        <v>248</v>
+      </c>
+      <c r="C18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="C19" t="s">
         <v>142</v>
       </c>
-      <c r="E17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="C18" t="s">
+      <c r="D19" t="s">
         <v>143</v>
       </c>
-      <c r="D18" t="s">
-        <v>144</v>
-      </c>
-      <c r="E18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" t="s">
-        <v>147</v>
-      </c>
-      <c r="C19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" t="s">
-        <v>149</v>
-      </c>
       <c r="E19" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" t="s">
         <v>148</v>
       </c>
-      <c r="D20" t="s">
-        <v>153</v>
-      </c>
       <c r="E20" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C21" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D21" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E21" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C22" t="s">
+        <v>156</v>
+      </c>
+      <c r="D22" t="s">
         <v>157</v>
       </c>
-      <c r="D22" t="s">
-        <v>168</v>
-      </c>
       <c r="E22" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B23" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" t="s">
         <v>167</v>
       </c>
-      <c r="D23" t="s">
-        <v>169</v>
-      </c>
       <c r="E23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D24" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
+        <v>166</v>
+      </c>
+      <c r="D26" t="s">
+        <v>176</v>
       </c>
       <c r="E26" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E27" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C28" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="E28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E29" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C30" t="s">
-        <v>191</v>
-      </c>
-      <c r="D30" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E30" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B31" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C31" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" t="s">
+        <v>193</v>
+      </c>
+      <c r="E31" t="s">
         <v>191</v>
-      </c>
-      <c r="E31" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E32" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B33" t="s">
+        <v>201</v>
+      </c>
+      <c r="C33" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>198</v>
+      </c>
+      <c r="B34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" t="s">
         <v>199</v>
       </c>
-      <c r="B33" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" t="s">
-        <v>191</v>
-      </c>
-      <c r="E33" t="s">
-        <v>200</v>
-      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A35:E35"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2223,364 +2327,500 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
         <v>204</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" t="s">
+        <v>206</v>
+      </c>
+      <c r="D8" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="C9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" t="s">
+        <v>208</v>
+      </c>
+      <c r="D11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="C13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" t="s">
+        <v>212</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" t="s">
         <v>213</v>
       </c>
-      <c r="D1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="C15" t="s">
         <v>214</v>
       </c>
-      <c r="D2" t="b">
+      <c r="D15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="B3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D3" t="b">
+    <row r="16" spans="1:5">
+      <c r="C16" t="s">
+        <v>215</v>
+      </c>
+      <c r="D16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" t="s">
+        <v>216</v>
+      </c>
+      <c r="D17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" t="s">
-        <v>214</v>
-      </c>
-      <c r="D4" t="b">
+    <row r="19" spans="3:5">
+      <c r="C19" t="s">
+        <v>218</v>
+      </c>
+      <c r="D19" t="s">
+        <v>220</v>
+      </c>
+      <c r="E19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>212</v>
-      </c>
-      <c r="B8" t="s">
-        <v>207</v>
-      </c>
-      <c r="C8" t="s">
-        <v>214</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" t="s">
-        <v>208</v>
-      </c>
-      <c r="C9" t="s">
-        <v>214</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>214</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C11" t="s">
-        <v>214</v>
-      </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C12" t="s">
-        <v>214</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" t="s">
-        <v>211</v>
-      </c>
-      <c r="C13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" t="s">
-        <v>215</v>
-      </c>
-      <c r="C14" t="s">
-        <v>222</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="B15" t="s">
-        <v>216</v>
-      </c>
-      <c r="C15" t="s">
-        <v>222</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="B16" t="s">
-        <v>217</v>
-      </c>
-      <c r="C16" t="s">
-        <v>222</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" t="s">
-        <v>218</v>
-      </c>
-      <c r="C17" t="s">
-        <v>222</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18" t="s">
+    <row r="20" spans="3:5">
+      <c r="C20" t="s">
         <v>219</v>
       </c>
-      <c r="C18" t="s">
-        <v>222</v>
-      </c>
-      <c r="D18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19" t="s">
+      <c r="D20" t="s">
         <v>220</v>
       </c>
-      <c r="C19" t="s">
-        <v>222</v>
-      </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20" t="s">
-        <v>221</v>
-      </c>
-      <c r="C20" t="s">
-        <v>222</v>
-      </c>
-      <c r="D20" t="b">
+      <c r="E20" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
         <v>224</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
         <v>226</v>
       </c>
-      <c r="C1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>225</v>
-      </c>
-      <c r="B2" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" t="b">
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
+        <v>227</v>
+      </c>
+      <c r="D6" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="B3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C3" t="b">
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" t="s">
+        <v>228</v>
+      </c>
+      <c r="D7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" t="b">
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" t="b">
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>214</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" t="s">
-        <v>230</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" t="s">
-        <v>231</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B8" t="s">
-        <v>233</v>
-      </c>
-      <c r="C8" t="b">
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>238</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>234</v>
-      </c>
-      <c r="B11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C11" t="b">
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D19" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>